<commit_message>
Upload May 10 2024
</commit_message>
<xml_diff>
--- a/Students-group.xlsx
+++ b/Students-group.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Student\2403.E0\sem1\1.LBEP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Student\2403.E0\sem1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA496A7-C5DB-46D5-87ED-D1F894E5CF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABDE20B-6407-4A4C-9632-B370A68A97DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Email</t>
   </si>
@@ -173,16 +173,35 @@
   </si>
   <si>
     <t>Ngô Tiến Phát</t>
+  </si>
+  <si>
+    <t>subgrid layout</t>
+  </si>
+  <si>
+    <t>new viewport unit</t>
+  </si>
+  <si>
+    <t>nesting layout</t>
+  </si>
+  <si>
+    <t>video, audio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,7 +216,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,9 +233,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -562,9 +583,10 @@
     <col min="1" max="1" width="32.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="31.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -586,8 +608,11 @@
         <v>18</v>
       </c>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -599,7 +624,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -611,7 +636,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -623,7 +648,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -635,19 +660,19 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -657,8 +682,11 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -669,7 +697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -680,7 +708,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -691,7 +719,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -702,18 +730,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -724,8 +752,11 @@
         <v>6</v>
       </c>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -737,7 +768,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -749,7 +780,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -761,7 +792,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -773,7 +804,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -785,7 +816,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -795,8 +826,11 @@
       <c r="C20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -807,7 +841,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -818,7 +852,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -829,7 +863,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -840,7 +874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>27</v>
       </c>

</xml_diff>